<commit_message>
Round up seconds in CellElapsedFormatter
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/ElapsedFormatTests.xlsx
+++ b/test-data/spreadsheet/ElapsedFormatTests.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyschott/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2383C6B-D02F-2B4E-9306-4DF0FAC13E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="0" windowWidth="20300" windowHeight="22840" tabRatio="500"/>
+    <workbookView xWindow="13500" yWindow="500" windowWidth="20300" windowHeight="22840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flags" sheetId="2" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
   <si>
     <t>s:m" @ hour "[hh]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -130,23 +147,19 @@
   <si>
     <t>Elapsed</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[h]\h m\m s\s</t>
+  </si>
+  <si>
+    <t>Elapsed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.00000000E+00"/>
-    <numFmt numFmtId="170" formatCode="dd\-mmm\-yyyy\ hh:mm:ss.000"/>
-    <numFmt numFmtId="171" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -163,6 +176,16 @@
     <font>
       <sz val="10"/>
       <name val="Lucida Sans Typewriter"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Sans Typewriter"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -220,10 +243,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -232,6 +255,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -554,23 +585,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="7"/>
+    <col min="1" max="1" width="10.6640625" style="7"/>
     <col min="2" max="2" width="17" style="8" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="1"/>
+    <col min="3" max="3" width="34.83203125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -581,7 +612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -589,7 +620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -598,7 +629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -610,7 +641,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -623,25 +653,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D215"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="2"/>
+    <col min="5" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -655,165 +685,165 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="str">
         <f t="shared" ref="A2:A6" si="0">TEXT(C2, B2)</f>
         <v>75:23:53.376</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="str">
         <f t="shared" si="0"/>
         <v>4523:53.376</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="str">
         <f t="shared" si="0"/>
         <v>271433.376</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>75:23:53.4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>4523:53.4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="str">
         <f t="shared" ref="A7" si="1">TEXT(C7, B7)</f>
         <v>271433.376</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="str">
         <f t="shared" ref="A8:A63" si="2">TEXT(C8, B8)</f>
-        <v>53:23 @ hour 75</v>
-      </c>
-      <c r="B8" s="10" t="s">
+        <v>53:23 @ hour 1293</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>53 secs and 4523 mins</v>
-      </c>
-      <c r="B9" s="10" t="s">
+        <v>53 secs and 77581 mins</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>It was 75 [yes, 75] hours and 23:53</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="str">
         <f t="shared" ref="A11:A20" si="3">TEXT(C11, B11)</f>
         <v>271433 [yes, 271433] seconds</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="str">
         <f t="shared" si="3"/>
         <v>2:3:4.000</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="2">
         <f>2/24+3/(24*60)+4/(24*60*60)</f>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -821,31 +851,31 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="str">
         <f t="shared" si="3"/>
         <v>123:4.000</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="11">
-        <f t="shared" ref="C13:C41" si="4">2/24+3/(24*60)+4/(24*60*60)</f>
+      <c r="C13" s="2">
+        <f t="shared" ref="C13:C21" si="4">2/24+3/(24*60)+4/(24*60*60)</f>
         <v>8.5462962962962963E-2</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="str">
         <f t="shared" si="3"/>
         <v>7384.000</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -853,15 +883,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="str">
         <f t="shared" si="3"/>
         <v>02:03:04.0</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -869,15 +899,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="3"/>
         <v>123:04.0</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -885,15 +915,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="3"/>
         <v>7384.000</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -901,15 +931,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>4:3 @ hour 02</v>
-      </c>
-      <c r="B18" s="10" t="s">
+        <v>4:3 @ hour 108</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -917,15 +947,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>4 secs and 123 mins</v>
-      </c>
-      <c r="B19" s="10" t="s">
+        <v>4 secs and 6480 mins</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -933,15 +963,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="3"/>
         <v>It was 2 [yes, 2] hours and 03:04</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -949,15 +979,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" ref="A21:A30" si="5">TEXT(C21, B21)</f>
         <v>7384 [yes, 7384] seconds</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -965,165 +995,165 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0:0:0.000</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="2">
         <v>0</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0:0.000</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="2">
         <v>0</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0.000</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="2">
         <v>0</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00:00:00.0</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="2">
         <v>0</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00:00.0</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="2">
         <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00.000</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="2">
         <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0:0 @ hour 00</v>
-      </c>
-      <c r="B28" s="10" t="s">
+        <v>0:0 @ hour 12</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="2">
         <v>0</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0 secs and 0 mins</v>
-      </c>
-      <c r="B29" s="10" t="s">
+        <v>0 secs and 720 mins</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="2">
         <v>0</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="5"/>
         <v>It was 0 [yes, 0] hours and 00:00</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="2">
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" ref="A31:A51" si="6">TEXT(C31, B31)</f>
         <v>0 [yes, 00] seconds</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="2">
         <v>0</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-2:3:4.000</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="2">
         <f>-(2/24+3/(24*60)+4/(24*60*60))</f>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1131,15 +1161,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-123:4.000</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="2">
         <f t="shared" ref="C33:C41" si="7">-(2/24+3/(24*60)+4/(24*60*60))</f>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1147,15 +1177,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384.000</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1163,15 +1193,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-02:03:04.0</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1179,15 +1209,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-123:04.0</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1195,15 +1225,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384.000</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1211,15 +1241,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-4:3 @ hour 02</v>
-      </c>
-      <c r="B38" s="10" t="s">
+        <v>-4:3 @ hour 108</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1227,15 +1257,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-4 secs and 123 mins</v>
-      </c>
-      <c r="B39" s="10" t="s">
+        <v>-4 secs and 6480 mins</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1243,15 +1273,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-It was 2 [yes, 2] hours and 03:04</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1259,15 +1289,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384 [yes, 7384] seconds</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1275,1298 +1305,1306 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-75:23:53.376</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-4523:53.376</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433.376</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-75:23:53.4</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-4523:53.4</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433.376</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-53:23 @ hour 75</v>
-      </c>
-      <c r="B48" s="10" t="s">
+        <v>-53:23 @ hour 1293</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-53 secs and 4523 mins</v>
-      </c>
-      <c r="B49" s="10" t="s">
+        <v>-53 secs and 77581 mins</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-It was 75 [yes, 75] hours and 23:53</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433 [yes, 271433] seconds</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="9" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4">
+        <v>0h 0m 9s</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="str">
         <f t="shared" ref="A64:A167" si="8">TEXT(C64, B64)</f>
         <v/>
       </c>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D167" s="7"/>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" s="9" t="str">
         <f t="shared" ref="A168:A184" si="9">TEXT(C168, B168)</f>
         <v/>
       </c>
       <c r="D168" s="7"/>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D169" s="7"/>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D170" s="7"/>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D171" s="7"/>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D172" s="7"/>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D173" s="7"/>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D174" s="7"/>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D182" s="7"/>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" s="9" t="str">
         <f t="shared" ref="A185:A204" si="10">TEXT(C185, B185)</f>
         <v/>
       </c>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D187" s="7"/>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D188" s="7"/>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D189" s="7"/>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D190" s="7"/>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D191" s="7"/>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D192" s="7"/>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D193" s="7"/>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D194" s="7"/>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D195" s="7"/>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D196" s="7"/>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D197" s="7"/>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A198" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D198" s="7"/>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D199" s="7"/>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D200" s="7"/>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D201" s="7"/>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D202" s="7"/>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D203" s="7"/>
     </row>
-    <row r="204" spans="1:4">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D204" s="7"/>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" s="9" t="str">
         <f t="shared" ref="A205:A215" si="11">TEXT(C205, B205)</f>
         <v/>
       </c>
       <c r="D205" s="7"/>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D206" s="7"/>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D207" s="7"/>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D208" s="7"/>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D209" s="7"/>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" s="9" t="str">
         <f t="shared" ref="A210" si="12">TEXT(C210, B210)</f>
         <v/>
       </c>
       <c r="D210" s="7"/>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D211" s="7"/>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D212" s="7"/>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D213" s="7"/>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D214" s="7"/>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -2574,7 +2612,6 @@
       <c r="D215" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[github-487] Round up seconds in CellElapsedFormatter. Thanks to Anthony Schott. This closes #487
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1911228 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/ElapsedFormatTests.xlsx
+++ b/test-data/spreadsheet/ElapsedFormatTests.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyschott/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2383C6B-D02F-2B4E-9306-4DF0FAC13E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="0" windowWidth="20300" windowHeight="22840" tabRatio="500"/>
+    <workbookView xWindow="13500" yWindow="500" windowWidth="20300" windowHeight="22840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flags" sheetId="2" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
   <si>
     <t>s:m" @ hour "[hh]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -130,23 +147,19 @@
   <si>
     <t>Elapsed</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[h]\h m\m s\s</t>
+  </si>
+  <si>
+    <t>Elapsed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.00000000E+00"/>
-    <numFmt numFmtId="170" formatCode="dd\-mmm\-yyyy\ hh:mm:ss.000"/>
-    <numFmt numFmtId="171" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -163,6 +176,16 @@
     <font>
       <sz val="10"/>
       <name val="Lucida Sans Typewriter"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Sans Typewriter"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -220,10 +243,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -232,6 +255,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -554,23 +585,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="7"/>
+    <col min="1" max="1" width="10.6640625" style="7"/>
     <col min="2" max="2" width="17" style="8" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="1"/>
+    <col min="3" max="3" width="34.83203125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -581,7 +612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -589,7 +620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -598,7 +629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -610,7 +641,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -623,25 +653,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D215"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="2"/>
+    <col min="5" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -655,165 +685,165 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="str">
         <f t="shared" ref="A2:A6" si="0">TEXT(C2, B2)</f>
         <v>75:23:53.376</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="str">
         <f t="shared" si="0"/>
         <v>4523:53.376</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="str">
         <f t="shared" si="0"/>
         <v>271433.376</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>75:23:53.4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>4523:53.4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="str">
         <f t="shared" ref="A7" si="1">TEXT(C7, B7)</f>
         <v>271433.376</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="str">
         <f t="shared" ref="A8:A63" si="2">TEXT(C8, B8)</f>
-        <v>53:23 @ hour 75</v>
-      </c>
-      <c r="B8" s="10" t="s">
+        <v>53:23 @ hour 1293</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>53 secs and 4523 mins</v>
-      </c>
-      <c r="B9" s="10" t="s">
+        <v>53 secs and 77581 mins</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>It was 75 [yes, 75] hours and 23:53</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="str">
         <f t="shared" ref="A11:A20" si="3">TEXT(C11, B11)</f>
         <v>271433 [yes, 271433] seconds</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="2">
         <v>3.1415899999999999</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="str">
         <f t="shared" si="3"/>
         <v>2:3:4.000</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="2">
         <f>2/24+3/(24*60)+4/(24*60*60)</f>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -821,31 +851,31 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="str">
         <f t="shared" si="3"/>
         <v>123:4.000</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="11">
-        <f t="shared" ref="C13:C41" si="4">2/24+3/(24*60)+4/(24*60*60)</f>
+      <c r="C13" s="2">
+        <f t="shared" ref="C13:C21" si="4">2/24+3/(24*60)+4/(24*60*60)</f>
         <v>8.5462962962962963E-2</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="str">
         <f t="shared" si="3"/>
         <v>7384.000</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -853,15 +883,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="str">
         <f t="shared" si="3"/>
         <v>02:03:04.0</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -869,15 +899,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="3"/>
         <v>123:04.0</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -885,15 +915,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="3"/>
         <v>7384.000</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -901,15 +931,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>4:3 @ hour 02</v>
-      </c>
-      <c r="B18" s="10" t="s">
+        <v>4:3 @ hour 108</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -917,15 +947,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>4 secs and 123 mins</v>
-      </c>
-      <c r="B19" s="10" t="s">
+        <v>4 secs and 6480 mins</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -933,15 +963,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="3"/>
         <v>It was 2 [yes, 2] hours and 03:04</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -949,15 +979,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" ref="A21:A30" si="5">TEXT(C21, B21)</f>
         <v>7384 [yes, 7384] seconds</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="2">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -965,165 +995,165 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0:0:0.000</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="2">
         <v>0</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0:0.000</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="2">
         <v>0</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0.000</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="2">
         <v>0</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00:00:00.0</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="2">
         <v>0</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00:00.0</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="2">
         <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00.000</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="2">
         <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0:0 @ hour 00</v>
-      </c>
-      <c r="B28" s="10" t="s">
+        <v>0:0 @ hour 12</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="2">
         <v>0</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0 secs and 0 mins</v>
-      </c>
-      <c r="B29" s="10" t="s">
+        <v>0 secs and 720 mins</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="2">
         <v>0</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="5"/>
         <v>It was 0 [yes, 0] hours and 00:00</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="2">
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" ref="A31:A51" si="6">TEXT(C31, B31)</f>
         <v>0 [yes, 00] seconds</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="2">
         <v>0</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-2:3:4.000</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="2">
         <f>-(2/24+3/(24*60)+4/(24*60*60))</f>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1131,15 +1161,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-123:4.000</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="2">
         <f t="shared" ref="C33:C41" si="7">-(2/24+3/(24*60)+4/(24*60*60))</f>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1147,15 +1177,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384.000</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1163,15 +1193,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-02:03:04.0</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1179,15 +1209,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-123:04.0</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1195,15 +1225,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384.000</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1211,15 +1241,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-4:3 @ hour 02</v>
-      </c>
-      <c r="B38" s="10" t="s">
+        <v>-4:3 @ hour 108</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1227,15 +1257,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-4 secs and 123 mins</v>
-      </c>
-      <c r="B39" s="10" t="s">
+        <v>-4 secs and 6480 mins</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1243,15 +1273,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-It was 2 [yes, 2] hours and 03:04</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1259,15 +1289,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384 [yes, 7384] seconds</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="2">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1275,1298 +1305,1306 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-75:23:53.376</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-4523:53.376</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433.376</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-75:23:53.4</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-4523:53.4</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433.376</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-53:23 @ hour 75</v>
-      </c>
-      <c r="B48" s="10" t="s">
+        <v>-53:23 @ hour 1293</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-53 secs and 4523 mins</v>
-      </c>
-      <c r="B49" s="10" t="s">
+        <v>-53 secs and 77581 mins</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-It was 75 [yes, 75] hours and 23:53</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433 [yes, 271433] seconds</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="2">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="9" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4">
+        <v>0h 0m 9s</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="str">
         <f t="shared" ref="A64:A167" si="8">TEXT(C64, B64)</f>
         <v/>
       </c>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D167" s="7"/>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" s="9" t="str">
         <f t="shared" ref="A168:A184" si="9">TEXT(C168, B168)</f>
         <v/>
       </c>
       <c r="D168" s="7"/>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D169" s="7"/>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D170" s="7"/>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D171" s="7"/>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D172" s="7"/>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D173" s="7"/>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D174" s="7"/>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D182" s="7"/>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" s="9" t="str">
         <f t="shared" ref="A185:A204" si="10">TEXT(C185, B185)</f>
         <v/>
       </c>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D187" s="7"/>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D188" s="7"/>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D189" s="7"/>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D190" s="7"/>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D191" s="7"/>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D192" s="7"/>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D193" s="7"/>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D194" s="7"/>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D195" s="7"/>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D196" s="7"/>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D197" s="7"/>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A198" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D198" s="7"/>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D199" s="7"/>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D200" s="7"/>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D201" s="7"/>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D202" s="7"/>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D203" s="7"/>
     </row>
-    <row r="204" spans="1:4">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D204" s="7"/>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" s="9" t="str">
         <f t="shared" ref="A205:A215" si="11">TEXT(C205, B205)</f>
         <v/>
       </c>
       <c r="D205" s="7"/>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D206" s="7"/>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D207" s="7"/>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D208" s="7"/>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D209" s="7"/>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" s="9" t="str">
         <f t="shared" ref="A210" si="12">TEXT(C210, B210)</f>
         <v/>
       </c>
       <c r="D210" s="7"/>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D211" s="7"/>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D212" s="7"/>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D213" s="7"/>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D214" s="7"/>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -2574,7 +2612,6 @@
       <c r="D215" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
undo last change due to broken test
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1911233 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/ElapsedFormatTests.xlsx
+++ b/test-data/spreadsheet/ElapsedFormatTests.xlsx
@@ -1,34 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyschott/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2383C6B-D02F-2B4E-9306-4DF0FAC13E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="500" windowWidth="20300" windowHeight="22840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13500" yWindow="0" windowWidth="20300" windowHeight="22840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Flags" sheetId="2" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -37,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
   <si>
     <t>s:m" @ hour "[hh]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -147,19 +130,23 @@
   <si>
     <t>Elapsed</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[h]\h m\m s\s</t>
-  </si>
-  <si>
-    <t>Elapsed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.00000000E+00"/>
+    <numFmt numFmtId="170" formatCode="dd\-mmm\-yyyy\ hh:mm:ss.000"/>
+    <numFmt numFmtId="171" formatCode="@"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -176,16 +163,6 @@
     <font>
       <sz val="10"/>
       <name val="Lucida Sans Typewriter"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lucida Sans Typewriter"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -243,10 +220,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -255,14 +232,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -585,23 +554,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="7"/>
+    <col min="1" max="1" width="10.7109375" style="7"/>
     <col min="2" max="2" width="17" style="8" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="10.6640625" style="1"/>
+    <col min="3" max="3" width="34.85546875" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -612,7 +581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -620,7 +589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -629,7 +598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -641,6 +610,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -653,25 +623,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="2"/>
+    <col min="5" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -685,165 +655,165 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" s="9" t="str">
         <f t="shared" ref="A2:A6" si="0">TEXT(C2, B2)</f>
         <v>75:23:53.376</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3" s="9" t="str">
         <f t="shared" si="0"/>
         <v>4523:53.376</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4" s="9" t="str">
         <f t="shared" si="0"/>
         <v>271433.376</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>75:23:53.4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>4523:53.4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="A7" s="9" t="str">
         <f t="shared" ref="A7" si="1">TEXT(C7, B7)</f>
         <v>271433.376</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8" s="9" t="str">
         <f t="shared" ref="A8:A63" si="2">TEXT(C8, B8)</f>
-        <v>53:23 @ hour 1293</v>
-      </c>
-      <c r="B8" s="9" t="s">
+        <v>53:23 @ hour 75</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="A9" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>53 secs and 77581 mins</v>
-      </c>
-      <c r="B9" s="9" t="s">
+        <v>53 secs and 4523 mins</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="A10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>It was 75 [yes, 75] hours and 23:53</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="A11" s="9" t="str">
         <f t="shared" ref="A11:A20" si="3">TEXT(C11, B11)</f>
         <v>271433 [yes, 271433] seconds</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="11">
         <v>3.1415899999999999</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="A12" s="9" t="str">
         <f t="shared" si="3"/>
         <v>2:3:4.000</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="11">
         <f>2/24+3/(24*60)+4/(24*60*60)</f>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -851,31 +821,31 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13" s="9" t="str">
         <f t="shared" si="3"/>
         <v>123:4.000</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="2">
-        <f t="shared" ref="C13:C21" si="4">2/24+3/(24*60)+4/(24*60*60)</f>
+      <c r="C13" s="11">
+        <f t="shared" ref="C13:C41" si="4">2/24+3/(24*60)+4/(24*60*60)</f>
         <v>8.5462962962962963E-2</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14" s="9" t="str">
         <f t="shared" si="3"/>
         <v>7384.000</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -883,15 +853,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15" s="9" t="str">
         <f t="shared" si="3"/>
         <v>02:03:04.0</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -899,15 +869,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
       <c r="A16" s="9" t="str">
         <f t="shared" si="3"/>
         <v>123:04.0</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -915,15 +885,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17" s="9" t="str">
         <f t="shared" si="3"/>
         <v>7384.000</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -931,15 +901,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>4:3 @ hour 108</v>
-      </c>
-      <c r="B18" s="9" t="s">
+        <v>4:3 @ hour 02</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -947,15 +917,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>4 secs and 6480 mins</v>
-      </c>
-      <c r="B19" s="9" t="s">
+        <v>4 secs and 123 mins</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -963,15 +933,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" s="9" t="str">
         <f t="shared" si="3"/>
         <v>It was 2 [yes, 2] hours and 03:04</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -979,15 +949,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21" s="9" t="str">
         <f t="shared" ref="A21:A30" si="5">TEXT(C21, B21)</f>
         <v>7384 [yes, 7384] seconds</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="11">
         <f t="shared" si="4"/>
         <v>8.5462962962962963E-2</v>
       </c>
@@ -995,165 +965,165 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0:0:0.000</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="11">
         <v>0</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0:0.000</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="11">
         <v>0</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" s="9" t="str">
         <f t="shared" si="5"/>
         <v>0.000</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="11">
         <v>0</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00:00:00.0</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="11">
         <v>0</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="A26" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00:00.0</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="11">
         <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="A27" s="9" t="str">
         <f t="shared" si="5"/>
         <v>00.000</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="11">
         <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4">
       <c r="A28" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0:0 @ hour 12</v>
-      </c>
-      <c r="B28" s="9" t="s">
+        <v>0:0 @ hour 00</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="11">
         <v>0</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0 secs and 720 mins</v>
-      </c>
-      <c r="B29" s="9" t="s">
+        <v>0 secs and 0 mins</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="11">
         <v>0</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4">
       <c r="A30" s="9" t="str">
         <f t="shared" si="5"/>
         <v>It was 0 [yes, 0] hours and 00:00</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="11">
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="A31" s="9" t="str">
         <f t="shared" ref="A31:A51" si="6">TEXT(C31, B31)</f>
         <v>0 [yes, 00] seconds</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="11">
         <v>0</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="A32" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-2:3:4.000</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="11">
         <f>-(2/24+3/(24*60)+4/(24*60*60))</f>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1161,15 +1131,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="A33" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-123:4.000</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="11">
         <f t="shared" ref="C33:C41" si="7">-(2/24+3/(24*60)+4/(24*60*60))</f>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1177,15 +1147,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4">
       <c r="A34" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384.000</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1193,15 +1163,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4">
       <c r="A35" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-02:03:04.0</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1209,15 +1179,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4">
       <c r="A36" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-123:04.0</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1225,15 +1195,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4">
       <c r="A37" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384.000</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1241,15 +1211,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4">
       <c r="A38" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-4:3 @ hour 108</v>
-      </c>
-      <c r="B38" s="9" t="s">
+        <v>-4:3 @ hour 02</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1257,15 +1227,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4">
       <c r="A39" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-4 secs and 6480 mins</v>
-      </c>
-      <c r="B39" s="9" t="s">
+        <v>-4 secs and 123 mins</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1273,15 +1243,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4">
       <c r="A40" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-It was 2 [yes, 2] hours and 03:04</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1289,15 +1259,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4">
       <c r="A41" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-7384 [yes, 7384] seconds</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="11">
         <f t="shared" si="7"/>
         <v>-8.5462962962962963E-2</v>
       </c>
@@ -1305,1306 +1275,1298 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4">
       <c r="A42" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-75:23:53.376</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4">
       <c r="A43" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-4523:53.376</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4">
       <c r="A44" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433.376</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4">
       <c r="A45" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-75:23:53.4</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4">
       <c r="A46" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-4523:53.4</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4">
       <c r="A47" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433.376</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4">
       <c r="A48" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-53:23 @ hour 1293</v>
-      </c>
-      <c r="B48" s="9" t="s">
+        <v>-53:23 @ hour 75</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4">
       <c r="A49" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>-53 secs and 77581 mins</v>
-      </c>
-      <c r="B49" s="9" t="s">
+        <v>-53 secs and 4523 mins</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4">
       <c r="A50" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-It was 75 [yes, 75] hours and 23:53</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4">
       <c r="A51" s="9" t="str">
         <f t="shared" si="6"/>
         <v>-271433 [yes, 271433] seconds</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="11">
         <v>-3.1415899999999999</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4">
       <c r="A52" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0h 0m 9s</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+        <v/>
+      </c>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4">
       <c r="A54" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4">
       <c r="A55" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4">
       <c r="A56" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4">
       <c r="A57" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4">
       <c r="A58" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4">
       <c r="A59" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4">
       <c r="A60" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4">
       <c r="A61" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4">
       <c r="A62" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4">
       <c r="A63" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4">
       <c r="A64" s="9" t="str">
         <f t="shared" ref="A64:A167" si="8">TEXT(C64, B64)</f>
         <v/>
       </c>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4">
       <c r="A65" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4">
       <c r="A66" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4">
       <c r="A67" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4">
       <c r="A68" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4">
       <c r="A69" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4">
       <c r="A70" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4">
       <c r="A71" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4">
       <c r="A72" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4">
       <c r="A73" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4">
       <c r="A74" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4">
       <c r="A75" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4">
       <c r="A76" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4">
       <c r="A77" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4">
       <c r="A78" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4">
       <c r="A79" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4">
       <c r="A80" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4">
       <c r="A81" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4">
       <c r="A82" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4">
       <c r="A83" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:4">
       <c r="A84" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:4">
       <c r="A85" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:4">
       <c r="A86" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:4">
       <c r="A87" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:4">
       <c r="A88" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:4">
       <c r="A89" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:4">
       <c r="A90" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:4">
       <c r="A91" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:4">
       <c r="A92" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:4">
       <c r="A93" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:4">
       <c r="A94" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:4">
       <c r="A95" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:4">
       <c r="A96" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:4">
       <c r="A97" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:4">
       <c r="A98" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:4">
       <c r="A99" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:4">
       <c r="A100" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:4">
       <c r="A101" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:4">
       <c r="A102" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:4">
       <c r="A103" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:4">
       <c r="A104" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:4">
       <c r="A105" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:4">
       <c r="A106" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:4">
       <c r="A107" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:4">
       <c r="A108" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:4">
       <c r="A109" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:4">
       <c r="A110" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:4">
       <c r="A111" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:4">
       <c r="A112" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:4">
       <c r="A113" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:4">
       <c r="A114" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:4">
       <c r="A115" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:4">
       <c r="A116" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:4">
       <c r="A117" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:4">
       <c r="A118" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:4">
       <c r="A119" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:4">
       <c r="A120" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:4">
       <c r="A121" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:4">
       <c r="A122" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:4">
       <c r="A123" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:4">
       <c r="A124" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:4">
       <c r="A125" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:4">
       <c r="A126" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:4">
       <c r="A127" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:4">
       <c r="A128" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:4">
       <c r="A129" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:4">
       <c r="A130" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:4">
       <c r="A131" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:4">
       <c r="A132" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:4">
       <c r="A133" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:4">
       <c r="A134" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:4">
       <c r="A135" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:4">
       <c r="A136" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:4">
       <c r="A137" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:4">
       <c r="A138" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:4">
       <c r="A139" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:4">
       <c r="A140" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:4">
       <c r="A141" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:4">
       <c r="A142" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:4">
       <c r="A143" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:4">
       <c r="A144" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4">
       <c r="A145" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4">
       <c r="A146" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4">
       <c r="A147" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:4">
       <c r="A148" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:4">
       <c r="A149" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:4">
       <c r="A150" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:4">
       <c r="A151" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:4">
       <c r="A152" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:4">
       <c r="A153" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:4">
       <c r="A154" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:4">
       <c r="A155" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:4">
       <c r="A156" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:4">
       <c r="A157" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:4">
       <c r="A158" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:4">
       <c r="A159" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:4">
       <c r="A160" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:4">
       <c r="A161" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:4">
       <c r="A162" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:4">
       <c r="A163" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:4">
       <c r="A164" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:4">
       <c r="A165" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:4">
       <c r="A166" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:4">
       <c r="A167" s="9" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D167" s="7"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:4">
       <c r="A168" s="9" t="str">
         <f t="shared" ref="A168:A184" si="9">TEXT(C168, B168)</f>
         <v/>
       </c>
       <c r="D168" s="7"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:4">
       <c r="A169" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D169" s="7"/>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:4">
       <c r="A170" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D170" s="7"/>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:4">
       <c r="A171" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D171" s="7"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:4">
       <c r="A172" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D172" s="7"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:4">
       <c r="A173" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D173" s="7"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:4">
       <c r="A174" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D174" s="7"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:4">
       <c r="A175" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:4">
       <c r="A176" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:4">
       <c r="A177" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:4">
       <c r="A178" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:4">
       <c r="A179" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:4">
       <c r="A180" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:4">
       <c r="A181" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:4">
       <c r="A182" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D182" s="7"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:4">
       <c r="A183" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:4">
       <c r="A184" s="9" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:4">
       <c r="A185" s="9" t="str">
         <f t="shared" ref="A185:A204" si="10">TEXT(C185, B185)</f>
         <v/>
       </c>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:4">
       <c r="A186" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:4">
       <c r="A187" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D187" s="7"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:4">
       <c r="A188" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D188" s="7"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:4">
       <c r="A189" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D189" s="7"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:4">
       <c r="A190" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D190" s="7"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:4">
       <c r="A191" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D191" s="7"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:4">
       <c r="A192" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D192" s="7"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:4">
       <c r="A193" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D193" s="7"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:4">
       <c r="A194" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D194" s="7"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:4">
       <c r="A195" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D195" s="7"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:4">
       <c r="A196" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D196" s="7"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:4">
       <c r="A197" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D197" s="7"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:4">
       <c r="A198" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D198" s="7"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:4">
       <c r="A199" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D199" s="7"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:4">
       <c r="A200" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D200" s="7"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:4">
       <c r="A201" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D201" s="7"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:4">
       <c r="A202" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D202" s="7"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:4">
       <c r="A203" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D203" s="7"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:4">
       <c r="A204" s="9" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="D204" s="7"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:4">
       <c r="A205" s="9" t="str">
         <f t="shared" ref="A205:A215" si="11">TEXT(C205, B205)</f>
         <v/>
       </c>
       <c r="D205" s="7"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:4">
       <c r="A206" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D206" s="7"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:4">
       <c r="A207" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D207" s="7"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:4">
       <c r="A208" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D208" s="7"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:4">
       <c r="A209" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D209" s="7"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:4">
       <c r="A210" s="9" t="str">
         <f t="shared" ref="A210" si="12">TEXT(C210, B210)</f>
         <v/>
       </c>
       <c r="D210" s="7"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:4">
       <c r="A211" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D211" s="7"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:4">
       <c r="A212" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D212" s="7"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:4">
       <c r="A213" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D213" s="7"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:4">
       <c r="A214" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="D214" s="7"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:4">
       <c r="A215" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -2612,6 +2574,7 @@
       <c r="D215" s="7"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>